<commit_message>
change 'image file name' to 'file' type
</commit_message>
<xml_diff>
--- a/images/image_schema_main_v0.1.xlsx
+++ b/images/image_schema_main_v0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/providen/Documents/EI/Projects/COPO-schemas/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zef22hak/development/COPO-schemas/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC5D95-1291-6243-8B48-91173B01EFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E199BB09-5874-ED41-AAF2-190F9D106673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35480" yWindow="-2600" windowWidth="33160" windowHeight="21400" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
+    <workbookView xWindow="32820" yWindow="500" windowWidth="33160" windowHeight="21100" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="457">
   <si>
     <t>component_name</t>
   </si>
@@ -1493,6 +1493,9 @@
   </si>
   <si>
     <t>Input must be  at least 25 characters.</t>
+  </si>
+  <si>
+    <t>file</t>
   </si>
 </sst>
 </file>
@@ -2518,8 +2521,8 @@
   <dimension ref="A1:P696"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A82" sqref="A82:XFD82"/>
+      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M83" sqref="M83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5697,7 +5700,7 @@
         <v>20</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>21</v>
+        <v>456</v>
       </c>
       <c r="N83" s="53"/>
       <c r="O83" s="41" t="s">

</xml_diff>